<commit_message>
Updated trip current test cases
</commit_message>
<xml_diff>
--- a/Test Data/TC_63797_Verify Trip Current Calculation.xlsx
+++ b/Test Data/TC_63797_Verify Trip Current Calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CAB6FA-CCD2-47A2-B5E6-541B1C3F1BA3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E02D31-4F70-43B7-B6A7-A83185C494F6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="56">
   <si>
     <t>Device</t>
   </si>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,6 +660,9 @@
         <v>328.8</v>
       </c>
       <c r="H1" s="5"/>
+      <c r="I1" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="L1"/>
     </row>
     <row r="2" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
@@ -678,6 +681,9 @@
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="8"/>
+      <c r="I2" s="13" t="s">
+        <v>54</v>
+      </c>
       <c r="L2"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -699,6 +705,9 @@
       </c>
       <c r="G3" s="1">
         <v>5</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="L3"/>
     </row>
@@ -919,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -957,6 +966,9 @@
         <v>494</v>
       </c>
       <c r="H1" s="3"/>
+      <c r="I1" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -977,6 +989,9 @@
       <c r="G2" s="8">
         <v>328.8</v>
       </c>
+      <c r="I2" s="13" t="s">
+        <v>54</v>
+      </c>
       <c r="J2" s="5"/>
       <c r="K2" s="12"/>
     </row>
@@ -999,6 +1014,9 @@
       </c>
       <c r="G3" s="1">
         <v>5</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="6"/>
@@ -1181,7 +1199,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>